<commit_message>
import data from CSV
</commit_message>
<xml_diff>
--- a/example data.xlsx
+++ b/example data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsopata/_projects/studies/PO_zad2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64E25DC9-4764-3246-9B4E-08BC9B9771FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A904C886-DE73-1E44-9479-4A86A7D0C97D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="74240" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{3A4948C0-49AB-884D-9D70-9DB96B59EF0E}"/>
+    <workbookView xWindow="77280" yWindow="1420" windowWidth="38400" windowHeight="21140" xr2:uid="{3A4948C0-49AB-884D-9D70-9DB96B59EF0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,9 +38,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>sin x * y. + exp(z)</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>LOG(X) / Y - TG(Z)</t>
   </si>
 </sst>
 </file>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83157E31-2FF2-7142-81CA-45066EAD0B0C}">
-  <dimension ref="B6:F30"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D2" sqref="D2:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -410,317 +410,399 @@
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f ca="1">RAND()</f>
+        <v>0.94694993508278169</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:C2" ca="1" si="0">RAND()</f>
+        <v>9.470394323316178E-2</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.52052533070861973</v>
+      </c>
+      <c r="D2">
+        <f ca="1">LOG(A2)/B2-TAN(C2)</f>
+        <v>-0.82322786419017002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f t="shared" ref="A3:C22" ca="1" si="1">RAND()</f>
+        <v>0.21945782405148773</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70525168168264563</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26751195282274565</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D22" ca="1" si="2">LOG(A3)/B3-TAN(C3)</f>
+        <v>-1.2080017521575379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32607681588029225</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52234601815374315</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93424504721462576</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="2"/>
+        <v>-2.284538999758071</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34759203363950109</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.1808123470296028E-3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6624460894838329E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-388.7431653162111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69703939583841223</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36408637358301843</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26487325008817275</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.70175606421487224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6810795601114426E-2</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.27225817209698855</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44366562149415012</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="2"/>
+        <v>-6.9926528263746413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4688853776715578</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31375639977607317</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75205157291139468</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.9838075165312761</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55425113771315548</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83203820851916233</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.12057189354113174</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.42919039990718766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34723055667611824</v>
+      </c>
       <c r="B10">
-        <v>0.82630842699999996</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.33628666819532205</v>
       </c>
       <c r="C10">
-        <v>0.54869639800000003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4519244641781619</v>
       </c>
       <c r="D10">
-        <v>0.114552399</v>
-      </c>
-      <c r="E10">
-        <v>1.524901931</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.8514738425845692</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70400034150831148</v>
+      </c>
       <c r="B11">
-        <v>0.40994185599999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83971275662451295</v>
       </c>
       <c r="C11">
-        <v>0.63354905100000003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.50404914771668519</v>
       </c>
       <c r="D11">
-        <v>0.67903099899999997</v>
-      </c>
-      <c r="E11">
-        <v>2.2244707469999998</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.73309471813087768</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.40044699195431532</v>
+      </c>
       <c r="B12">
-        <v>0.77503770999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.23026065156387288</v>
       </c>
       <c r="C12">
-        <v>0.46413915100000003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4456329370693064</v>
       </c>
       <c r="D12">
-        <v>0.31819127600000002</v>
-      </c>
-      <c r="E12">
-        <v>1.699417301</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-2.2037892054167951</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.63415161673617682</v>
+      </c>
       <c r="B13">
-        <v>0.542992751</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.17719520789093435</v>
       </c>
       <c r="C13">
-        <v>0.786261082</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.20404630989939276</v>
       </c>
       <c r="D13">
-        <v>0.61243024400000001</v>
-      </c>
-      <c r="E13">
-        <v>2.251171104</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.3232480223157013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.61925017495277745</v>
+      </c>
       <c r="B14">
-        <v>0.93087485199999997</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3395710526808039</v>
       </c>
       <c r="C14">
-        <v>0.88914295200000004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.40958887849073633</v>
       </c>
       <c r="D14">
-        <v>0.49711053399999999</v>
-      </c>
-      <c r="E14">
-        <v>2.3571837069999999</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.0470742061619935</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91585476996526427</v>
+      </c>
       <c r="B15">
-        <v>0.65631615399999998</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21090469743196494</v>
       </c>
       <c r="C15">
-        <v>0.74117147100000003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.97169750748110917</v>
       </c>
       <c r="D15">
-        <v>0.905906239</v>
-      </c>
-      <c r="E15">
-        <v>2.9264377760000002</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.6455245630327329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70636702301619159</v>
+      </c>
       <c r="B16">
-        <v>4.4077343999999997E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87785336307129469</v>
       </c>
       <c r="C16">
-        <v>3.5014352999999998E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58114378954737878</v>
       </c>
       <c r="D16">
-        <v>0.81661159699999997</v>
-      </c>
-      <c r="E16">
-        <v>2.2643623289999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.82878028839447448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.28713714865385442</v>
+      </c>
       <c r="B17">
-        <v>0.53341720199999998</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.86945046338509513</v>
       </c>
       <c r="C17">
-        <v>0.59766930900000004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69228590686875524</v>
       </c>
       <c r="D17">
-        <v>0.52062324999999998</v>
-      </c>
-      <c r="E17">
-        <v>1.9869784539999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.4524658577517411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.90852237200010044</v>
+      </c>
       <c r="B18">
-        <v>0.91389357000000004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93216239498035836</v>
       </c>
       <c r="C18">
-        <v>0.26338064500000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4186442461601616</v>
       </c>
       <c r="D18">
-        <v>0.91156996800000001</v>
-      </c>
-      <c r="E18">
-        <v>2.6967937200000001</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.48964387717175972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.33079738540967496</v>
+      </c>
       <c r="B19">
-        <v>0.81404986000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.78848253355819331</v>
       </c>
       <c r="C19">
-        <v>0.50490008099999995</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4521349881788298</v>
       </c>
       <c r="D19">
-        <v>0.59458966000000002</v>
-      </c>
-      <c r="E19">
-        <v>2.1793866579999999</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.0950106475623562</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.11152040663896479</v>
+      </c>
       <c r="B20">
-        <v>0.51799503099999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68045333655113638</v>
       </c>
       <c r="C20">
-        <v>0.76075166299999997</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31612397971356421</v>
       </c>
       <c r="D20">
-        <v>0.257085852</v>
-      </c>
-      <c r="E20">
-        <v>1.669834104</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.7271093642279349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10137343825417022</v>
+      </c>
       <c r="B21">
-        <v>0.83455742600000005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32869373748689179</v>
       </c>
       <c r="C21">
-        <v>0.88508398200000005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.43702390497632537</v>
       </c>
       <c r="D21">
-        <v>9.1525606999999995E-2</v>
-      </c>
-      <c r="E21">
-        <v>1.7516915310000001</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-3.491472274372478</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.94662911725307441</v>
+      </c>
       <c r="B22">
-        <v>0.735834714</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.35252667173809271</v>
       </c>
       <c r="C22">
-        <v>0.79230334700000005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.50330930723629974</v>
       </c>
       <c r="D22">
-        <v>0.80020818900000001</v>
-      </c>
-      <c r="E22">
-        <v>2.7578031799999998</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>0.30268204999999998</v>
-      </c>
-      <c r="C23">
-        <v>0.86399684200000004</v>
-      </c>
-      <c r="D23">
-        <v>0.970508288</v>
-      </c>
-      <c r="E23">
-        <v>2.896827026</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>0.212188653</v>
-      </c>
-      <c r="C24">
-        <v>0.85931091400000004</v>
-      </c>
-      <c r="D24">
-        <v>0.425617627</v>
-      </c>
-      <c r="E24">
-        <v>1.71150628</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>0.838560792</v>
-      </c>
-      <c r="C25">
-        <v>0.60562572800000003</v>
-      </c>
-      <c r="D25">
-        <v>0.38459202100000001</v>
-      </c>
-      <c r="E25">
-        <v>1.919407662</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26">
-        <v>0.74615975899999998</v>
-      </c>
-      <c r="C26">
-        <v>4.8584571999999999E-2</v>
-      </c>
-      <c r="D26">
-        <v>0.812725331</v>
-      </c>
-      <c r="E26">
-        <v>2.2870230029999998</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27">
-        <v>0.95945559400000002</v>
-      </c>
-      <c r="C27">
-        <v>0.57992268800000002</v>
-      </c>
-      <c r="D27">
-        <v>0.76637229299999998</v>
-      </c>
-      <c r="E27">
-        <v>2.6268320869999999</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28">
-        <v>0.96919294099999997</v>
-      </c>
-      <c r="C28">
-        <v>7.0758029E-2</v>
-      </c>
-      <c r="D28">
-        <v>0.16413697899999999</v>
-      </c>
-      <c r="E28">
-        <v>1.236710703</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29">
-        <v>0.15903916500000001</v>
-      </c>
-      <c r="C29">
-        <v>0.5980799</v>
-      </c>
-      <c r="D29">
-        <v>0.35782942899999998</v>
-      </c>
-      <c r="E29">
-        <v>1.524939303</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30">
-        <v>0.17833622700000001</v>
-      </c>
-      <c r="C30">
-        <v>0.97151275699999995</v>
-      </c>
-      <c r="D30">
-        <v>0.435408032</v>
-      </c>
-      <c r="E30">
-        <v>1.7179325940000001</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.61817700231712669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>